<commit_message>
fix error, add gp
</commit_message>
<xml_diff>
--- a/Docs/simple_AFO_results.xlsx
+++ b/Docs/simple_AFO_results.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="12270" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18120" windowHeight="12270"/>
   </bookViews>
   <sheets>
-    <sheet name="1 dim sensor" sheetId="1" r:id="rId1"/>
-    <sheet name="08-21-Aug-26 axisdim-3" sheetId="4" r:id="rId2"/>
-    <sheet name="09-19-Sep-55 axisdim-1" sheetId="5" r:id="rId3"/>
-    <sheet name="2 dim sensor" sheetId="2" r:id="rId4"/>
+    <sheet name="09-19-Sep-07 axisdim-1" sheetId="6" r:id="rId1"/>
+    <sheet name="09-19-Sep-55 axisdim-1" sheetId="5" r:id="rId2"/>
+    <sheet name="1 dim sensor" sheetId="1" r:id="rId3"/>
+    <sheet name="08-21-Aug-26 axisdim-3" sheetId="4" r:id="rId4"/>
+    <sheet name="2 dim sensor" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,6 +25,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>error x</t>
+  </si>
+  <si>
+    <t>std error x</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1253,7 +1271,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1549,7 +1566,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1667,7 +1683,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3823,6 +3838,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-43.18219183812603</v>
+      </c>
+      <c r="B2">
+        <v>-15.955414473921508</v>
+      </c>
+      <c r="C2">
+        <v>2.4307361496494679</v>
+      </c>
+      <c r="D2">
+        <v>0.93710359333166482</v>
+      </c>
+      <c r="E2">
+        <v>0.81987961728545233</v>
+      </c>
+      <c r="F2">
+        <v>0.70867778341221477</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-36.355190434214464</v>
+      </c>
+      <c r="B3">
+        <v>-1.9969211471969956</v>
+      </c>
+      <c r="C3">
+        <v>1.9694200179546981</v>
+      </c>
+      <c r="D3">
+        <v>1.9531553851668959</v>
+      </c>
+      <c r="E3">
+        <v>0.4434368298635063</v>
+      </c>
+      <c r="F3">
+        <v>0.92686799357871741</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-26.483272871817359</v>
+      </c>
+      <c r="B4">
+        <v>-30.733876966677389</v>
+      </c>
+      <c r="C4">
+        <v>1.653694853628886</v>
+      </c>
+      <c r="D4">
+        <v>1.7240972272975064</v>
+      </c>
+      <c r="E4">
+        <v>1.0625628305014143</v>
+      </c>
+      <c r="F4">
+        <v>0.5064017217406952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-14.083710212183425</v>
+      </c>
+      <c r="B5">
+        <v>-35.504383916645203</v>
+      </c>
+      <c r="C5">
+        <v>0.72164144145003384</v>
+      </c>
+      <c r="D5">
+        <v>1.9923241327096561</v>
+      </c>
+      <c r="E5">
+        <v>0.69792328415649563</v>
+      </c>
+      <c r="F5">
+        <v>0.64116358210871172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.6588162385026154E-2</v>
+      </c>
+      <c r="B6">
+        <v>-29.074518909751795</v>
+      </c>
+      <c r="C6">
+        <v>1.2774447363034482</v>
+      </c>
+      <c r="D6">
+        <v>1.3423079875105806</v>
+      </c>
+      <c r="E6">
+        <v>0.80474110397402587</v>
+      </c>
+      <c r="F6">
+        <v>0.39974419355763535</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14.885407273364828</v>
+      </c>
+      <c r="B7">
+        <v>3.5994845598548943</v>
+      </c>
+      <c r="C7">
+        <v>2.8283191843755704</v>
+      </c>
+      <c r="D7">
+        <v>3.8991135388225606</v>
+      </c>
+      <c r="E7">
+        <v>0.59222440529149067</v>
+      </c>
+      <c r="F7">
+        <v>1.233542588790274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>25.774086920076364</v>
+      </c>
+      <c r="B8">
+        <v>6.1978169679871886</v>
+      </c>
+      <c r="C8">
+        <v>4.2609918273029299</v>
+      </c>
+      <c r="D8">
+        <v>3.962753927730688</v>
+      </c>
+      <c r="E8">
+        <v>0.7080075258114662</v>
+      </c>
+      <c r="F8">
+        <v>1.4909841351048236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-43.18219183812603</v>
+      </c>
+      <c r="B1">
+        <v>4.4160861862705616</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-36.355190434214464</v>
+      </c>
+      <c r="B2">
+        <v>3.104385533091417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-26.483272871817363</v>
+      </c>
+      <c r="B3">
+        <v>3.1213095997226361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-14.083710212183425</v>
+      </c>
+      <c r="B4">
+        <v>1.038606185388991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.6588162385026154E-2</v>
+      </c>
+      <c r="B5">
+        <v>0.48607077141861077</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>14.885407273364828</v>
+      </c>
+      <c r="B6">
+        <v>1.2781732722051604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25.774086920076368</v>
+      </c>
+      <c r="B7">
+        <v>3.6498975432453129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3936,7 +4198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -4051,78 +4313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>-43.18219183812603</v>
-      </c>
-      <c r="B1">
-        <v>4.4160861862705616</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>-36.355190434214464</v>
-      </c>
-      <c r="B2">
-        <v>3.104385533091417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>-26.483272871817363</v>
-      </c>
-      <c r="B3">
-        <v>3.1213095997226361</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-14.083710212183425</v>
-      </c>
-      <c r="B4">
-        <v>1.038606185388991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5.6588162385026154E-2</v>
-      </c>
-      <c r="B5">
-        <v>0.48607077141861077</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>14.885407273364828</v>
-      </c>
-      <c r="B6">
-        <v>1.2781732722051604</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>25.774086920076368</v>
-      </c>
-      <c r="B7">
-        <v>3.6498975432453129</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>

</xml_diff>